<commit_message>
fix embryo import dan test logic
</commit_message>
<xml_diff>
--- a/storage/app/public/form_import/form_import_embryo.xlsx
+++ b/storage/app/public/form_import/form_import_embryo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10119"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/socfindo/socfin_tcsawit/storage/app/public/form_import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aldhi/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F6AC1E-100C-0E42-ACB9-AF21BE46E422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FB70DF-15D3-9D48-881F-55C2A96FB722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="22100" windowWidth="40960" windowHeight="24460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17580" yWindow="28700" windowWidth="27720" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>21/12/2023</t>
   </si>
   <si>
-    <t>ID Worker</t>
-  </si>
-  <si>
     <t>Jlh Botol</t>
   </si>
   <si>
@@ -63,13 +60,16 @@
   </si>
   <si>
     <t>Sub Culture</t>
+  </si>
+  <si>
+    <t>&lt;end&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -81,16 +81,29 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -98,14 +111,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,107 +448,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E47813-669A-4B4E-A009-96C1097A77F5}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="5" max="5" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>100</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>200</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
+      <c r="F3" s="2">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>15</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="G3">
-        <v>27</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>